<commit_message>
update graphs visualization parameters
</commit_message>
<xml_diff>
--- a/archived/RMSE_Tempalte.xlsx
+++ b/archived/RMSE_Tempalte.xlsx
@@ -9,15 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="ALL(2001)" sheetId="1" r:id="rId1"/>
     <sheet name="ALL(2002)" sheetId="6" r:id="rId2"/>
     <sheet name="Sheet1" sheetId="5" r:id="rId3"/>
-    <sheet name="Forecasting2008-2009" sheetId="7" r:id="rId4"/>
-    <sheet name="Forcasting2001" sheetId="8" r:id="rId5"/>
-    <sheet name="Forecasting2020" sheetId="9" r:id="rId6"/>
+    <sheet name="Forecasting2008-2009_BP" sheetId="11" r:id="rId4"/>
+    <sheet name="Forecasting2008-2009" sheetId="7" r:id="rId5"/>
+    <sheet name="Forcasting2001_BP" sheetId="10" r:id="rId6"/>
+    <sheet name="Forcasting2001" sheetId="8" r:id="rId7"/>
+    <sheet name="Forecasting2020" sheetId="9" r:id="rId8"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="416" uniqueCount="43">
   <si>
     <t>Forecast Horizon</t>
   </si>
@@ -410,7 +412,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="79">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -559,22 +561,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -583,50 +570,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -644,11 +589,403 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="75">
+  <dxfs count="107">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -1720,69 +2057,69 @@
     <col min="1" max="1" width="10.42578125" style="3" customWidth="1"/>
     <col min="2" max="2" width="5.5703125" style="4" customWidth="1"/>
     <col min="3" max="5" width="8.85546875" style="4" customWidth="1"/>
-    <col min="6" max="6" width="8.85546875" style="73" customWidth="1"/>
+    <col min="6" max="6" width="8.85546875" style="54" customWidth="1"/>
     <col min="7" max="15" width="8.85546875" style="4" customWidth="1"/>
     <col min="16" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="76"/>
-      <c r="B1" s="73"/>
-      <c r="C1" s="73"/>
-      <c r="D1" s="73"/>
-      <c r="E1" s="73"/>
-      <c r="G1" s="73"/>
-      <c r="H1" s="73"/>
-      <c r="I1" s="73"/>
-      <c r="J1" s="73"/>
-      <c r="K1" s="73"/>
-      <c r="L1" s="73"/>
-      <c r="M1" s="73"/>
-      <c r="N1" s="73"/>
-      <c r="O1" s="73"/>
-      <c r="P1" s="76"/>
-      <c r="Q1" s="76"/>
+      <c r="A1" s="57"/>
+      <c r="B1" s="54"/>
+      <c r="C1" s="54"/>
+      <c r="D1" s="54"/>
+      <c r="E1" s="54"/>
+      <c r="G1" s="54"/>
+      <c r="H1" s="54"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="54"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="57"/>
+      <c r="Q1" s="57"/>
     </row>
     <row r="2" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="53" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="59" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="66"/>
-      <c r="G2" s="59" t="s">
+      <c r="F2" s="61"/>
+      <c r="G2" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="H2" s="66"/>
-      <c r="I2" s="59" t="s">
+      <c r="H2" s="61"/>
+      <c r="I2" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="J2" s="66"/>
-      <c r="K2" s="59" t="s">
+      <c r="J2" s="61"/>
+      <c r="K2" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="L2" s="66"/>
-      <c r="M2" s="59" t="s">
+      <c r="L2" s="61"/>
+      <c r="M2" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="N2" s="66"/>
+      <c r="N2" s="61"/>
       <c r="O2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="P2" s="76"/>
-      <c r="Q2" s="76"/>
+      <c r="P2" s="57"/>
+      <c r="Q2" s="57"/>
     </row>
     <row r="3" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="75"/>
       <c r="C3" s="44" t="s">
         <v>42</v>
       </c>
@@ -1820,11 +2157,11 @@
         <v>2</v>
       </c>
       <c r="O3" s="21"/>
-      <c r="P3" s="76"/>
-      <c r="Q3" s="76"/>
+      <c r="P3" s="57"/>
+      <c r="Q3" s="57"/>
     </row>
     <row r="4" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="7">
@@ -1869,11 +2206,11 @@
       <c r="O4" s="27">
         <v>1.04</v>
       </c>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="76"/>
+      <c r="P4" s="57"/>
+      <c r="Q4" s="57"/>
     </row>
     <row r="5" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="51"/>
+      <c r="A5" s="71"/>
       <c r="B5" s="4">
         <v>1</v>
       </c>
@@ -1916,11 +2253,11 @@
       <c r="O5" s="27">
         <v>0.99</v>
       </c>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="76"/>
+      <c r="P5" s="57"/>
+      <c r="Q5" s="57"/>
     </row>
     <row r="6" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="4">
         <v>2</v>
       </c>
@@ -1963,11 +2300,11 @@
       <c r="O6" s="27">
         <v>0.78</v>
       </c>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="76"/>
+      <c r="P6" s="57"/>
+      <c r="Q6" s="57"/>
     </row>
     <row r="7" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="4">
         <v>3</v>
       </c>
@@ -2010,11 +2347,11 @@
       <c r="O7" s="27">
         <v>1.43</v>
       </c>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="76"/>
+      <c r="P7" s="57"/>
+      <c r="Q7" s="57"/>
     </row>
     <row r="8" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="14">
         <v>4</v>
       </c>
@@ -2057,50 +2394,50 @@
       <c r="O8" s="31">
         <v>1.1599999999999999</v>
       </c>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="76"/>
+      <c r="P8" s="57"/>
+      <c r="Q8" s="57"/>
     </row>
     <row r="9" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F9" s="4"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="76"/>
+      <c r="P9" s="57"/>
+      <c r="Q9" s="57"/>
     </row>
     <row r="10" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="60" t="s">
+      <c r="A10" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B10" s="66"/>
-      <c r="C10" s="59" t="s">
+      <c r="B10" s="61"/>
+      <c r="C10" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="66"/>
-      <c r="E10" s="59" t="s">
+      <c r="D10" s="61"/>
+      <c r="E10" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="66"/>
-      <c r="G10" s="59" t="s">
+      <c r="F10" s="61"/>
+      <c r="G10" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="66"/>
-      <c r="I10" s="59" t="s">
+      <c r="H10" s="61"/>
+      <c r="I10" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="J10" s="66"/>
-      <c r="K10" s="59" t="s">
+      <c r="J10" s="61"/>
+      <c r="K10" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="66"/>
-      <c r="M10" s="59" t="s">
+      <c r="L10" s="61"/>
+      <c r="M10" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="N10" s="60"/>
+      <c r="N10" s="62"/>
       <c r="O10"/>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="61" t="s">
+      <c r="A11" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B11" s="62"/>
+      <c r="B11" s="64"/>
       <c r="C11" s="48" t="s">
         <v>42</v>
       </c>
@@ -2140,7 +2477,7 @@
       <c r="O11"/>
     </row>
     <row r="12" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="63" t="s">
+      <c r="A12" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="22">
@@ -2185,7 +2522,7 @@
       <c r="O12"/>
     </row>
     <row r="13" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="64"/>
+      <c r="A13" s="68"/>
       <c r="B13" s="26">
         <v>1</v>
       </c>
@@ -2228,7 +2565,7 @@
       <c r="O13"/>
     </row>
     <row r="14" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="26">
         <v>2</v>
       </c>
@@ -2271,7 +2608,7 @@
       <c r="O14"/>
     </row>
     <row r="15" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="26">
         <v>3</v>
       </c>
@@ -2314,7 +2651,7 @@
       <c r="O15"/>
     </row>
     <row r="16" spans="1:17" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="65"/>
+      <c r="A16" s="69"/>
       <c r="B16" s="30">
         <v>4</v>
       </c>
@@ -2374,26 +2711,26 @@
       <c r="O17"/>
     </row>
     <row r="18" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="60" t="s">
+      <c r="A18" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B18" s="66"/>
-      <c r="C18" s="59" t="s">
+      <c r="B18" s="61"/>
+      <c r="C18" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="D18" s="66"/>
-      <c r="E18" s="59" t="s">
+      <c r="D18" s="61"/>
+      <c r="E18" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="F18" s="66"/>
-      <c r="G18" s="59" t="s">
+      <c r="F18" s="61"/>
+      <c r="G18" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="H18" s="66"/>
-      <c r="I18" s="59" t="s">
+      <c r="H18" s="61"/>
+      <c r="I18" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="J18" s="60"/>
+      <c r="J18" s="62"/>
       <c r="K18" s="45" t="s">
         <v>3</v>
       </c>
@@ -2403,10 +2740,10 @@
       <c r="O18"/>
     </row>
     <row r="19" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="61" t="s">
+      <c r="A19" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="62"/>
+      <c r="B19" s="64"/>
       <c r="C19" s="21" t="s">
         <v>42</v>
       </c>
@@ -2440,7 +2777,7 @@
       <c r="O19"/>
     </row>
     <row r="20" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="63" t="s">
+      <c r="A20" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B20" s="36">
@@ -2479,7 +2816,7 @@
       <c r="O20"/>
     </row>
     <row r="21" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="64"/>
+      <c r="A21" s="68"/>
       <c r="B21" s="38">
         <v>1</v>
       </c>
@@ -2516,7 +2853,7 @@
       <c r="O21"/>
     </row>
     <row r="22" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
+      <c r="A22" s="68"/>
       <c r="B22" s="38">
         <v>2</v>
       </c>
@@ -2553,7 +2890,7 @@
       <c r="O22"/>
     </row>
     <row r="23" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
+      <c r="A23" s="68"/>
       <c r="B23" s="38">
         <v>3</v>
       </c>
@@ -2590,7 +2927,7 @@
       <c r="O23"/>
     </row>
     <row r="24" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="65"/>
+      <c r="A24" s="69"/>
       <c r="B24" s="40">
         <v>4</v>
       </c>
@@ -2627,42 +2964,58 @@
       <c r="O24"/>
     </row>
     <row r="25" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="76"/>
-      <c r="B25" s="73"/>
-      <c r="C25" s="73"/>
-      <c r="D25" s="73"/>
-      <c r="E25" s="73"/>
-      <c r="G25" s="73"/>
-      <c r="H25" s="73"/>
-      <c r="I25" s="73"/>
-      <c r="J25" s="73"/>
-      <c r="K25" s="73"/>
+      <c r="A25" s="57"/>
+      <c r="B25" s="54"/>
+      <c r="C25" s="54"/>
+      <c r="D25" s="54"/>
+      <c r="E25" s="54"/>
+      <c r="G25" s="54"/>
+      <c r="H25" s="54"/>
+      <c r="I25" s="54"/>
+      <c r="J25" s="54"/>
+      <c r="K25" s="54"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
     </row>
     <row r="26" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D26" s="73"/>
+      <c r="D26" s="54"/>
       <c r="L26" s="3"/>
       <c r="M26" s="3"/>
       <c r="N26" s="3"/>
       <c r="O26" s="3"/>
     </row>
     <row r="27" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D27" s="73"/>
+      <c r="D27" s="54"/>
     </row>
     <row r="28" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D28" s="73"/>
+      <c r="D28" s="54"/>
     </row>
     <row r="29" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D29" s="73"/>
+      <c r="D29" s="54"/>
     </row>
     <row r="30" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D30" s="73"/>
+      <c r="D30" s="54"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="A20:A24"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="A12:A16"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
     <mergeCell ref="G10:H10"/>
     <mergeCell ref="I10:J10"/>
     <mergeCell ref="K10:L10"/>
@@ -2671,93 +3024,77 @@
     <mergeCell ref="E18:F18"/>
     <mergeCell ref="G18:H18"/>
     <mergeCell ref="I18:J18"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="A20:A24"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="A12:A16"/>
-    <mergeCell ref="C10:D10"/>
     <mergeCell ref="E10:F10"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A18:B18"/>
   </mergeCells>
   <conditionalFormatting sqref="E4:F4 C12:N16 C5:O8 C21:J24">
-    <cfRule type="cellIs" dxfId="74" priority="17" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="73" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="106" priority="17" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="105" priority="18" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C4:D4">
-    <cfRule type="cellIs" dxfId="72" priority="15" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="71" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="104" priority="15" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="103" priority="16" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4:H4">
-    <cfRule type="cellIs" dxfId="70" priority="13" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="69" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="102" priority="13" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="101" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:J4">
-    <cfRule type="cellIs" dxfId="68" priority="11" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="67" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="100" priority="11" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="99" priority="12" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M4:N4">
-    <cfRule type="cellIs" dxfId="66" priority="9" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="65" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="98" priority="9" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="97" priority="10" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E20:J20">
-    <cfRule type="cellIs" dxfId="64" priority="3" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="96" priority="3" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="95" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O4">
-    <cfRule type="cellIs" dxfId="62" priority="1" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="61" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="94" priority="1" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="93" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K4:L4">
-    <cfRule type="cellIs" dxfId="60" priority="7" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="59" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="92" priority="7" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="91" priority="8" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C20:D20">
-    <cfRule type="cellIs" dxfId="58" priority="5" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="57" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="90" priority="5" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="89" priority="6" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2783,62 +3120,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="57" t="s">
+      <c r="A1" s="74" t="s">
         <v>27</v>
       </c>
-      <c r="B1" s="57"/>
-      <c r="C1" s="57"/>
-      <c r="D1" s="57"/>
-      <c r="E1" s="57"/>
-      <c r="F1" s="57"/>
-      <c r="G1" s="57"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="57"/>
-      <c r="J1" s="57"/>
-      <c r="K1" s="57"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="57"/>
-      <c r="N1" s="57"/>
-      <c r="O1" s="57"/>
+      <c r="B1" s="74"/>
+      <c r="C1" s="74"/>
+      <c r="D1" s="74"/>
+      <c r="E1" s="74"/>
+      <c r="F1" s="74"/>
+      <c r="G1" s="74"/>
+      <c r="H1" s="74"/>
+      <c r="I1" s="74"/>
+      <c r="J1" s="74"/>
+      <c r="K1" s="74"/>
+      <c r="L1" s="74"/>
+      <c r="M1" s="74"/>
+      <c r="N1" s="74"/>
+      <c r="O1" s="74"/>
     </row>
     <row r="2" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="54" t="s">
+      <c r="A2" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="55"/>
-      <c r="C2" s="54" t="s">
+      <c r="B2" s="66"/>
+      <c r="C2" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="55"/>
-      <c r="E2" s="53" t="s">
+      <c r="D2" s="66"/>
+      <c r="E2" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="F2" s="55"/>
-      <c r="G2" s="53" t="s">
+      <c r="F2" s="66"/>
+      <c r="G2" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="H2" s="55"/>
-      <c r="I2" s="53" t="s">
+      <c r="H2" s="66"/>
+      <c r="I2" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="J2" s="55"/>
-      <c r="K2" s="54" t="s">
+      <c r="J2" s="66"/>
+      <c r="K2" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="L2" s="55"/>
-      <c r="M2" s="53" t="s">
+      <c r="L2" s="66"/>
+      <c r="M2" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="N2" s="55"/>
-      <c r="O2" s="53" t="s">
+      <c r="N2" s="66"/>
+      <c r="O2" s="65" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="57" t="s">
+      <c r="A3" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="58"/>
+      <c r="B3" s="75"/>
       <c r="C3" s="5" t="s">
         <v>2</v>
       </c>
@@ -2875,10 +3212,10 @@
       <c r="N3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="O3" s="56"/>
+      <c r="O3" s="77"/>
     </row>
     <row r="4" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="50" t="s">
+      <c r="A4" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="18">
@@ -2913,7 +3250,7 @@
       </c>
     </row>
     <row r="5" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="67"/>
+      <c r="A5" s="76"/>
       <c r="B5" s="19">
         <v>1</v>
       </c>
@@ -2958,7 +3295,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="67"/>
+      <c r="A6" s="76"/>
       <c r="B6" s="19">
         <v>2</v>
       </c>
@@ -3003,7 +3340,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
+      <c r="A7" s="76"/>
       <c r="B7" s="19">
         <v>3</v>
       </c>
@@ -3048,7 +3385,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="52"/>
+      <c r="A8" s="72"/>
       <c r="B8" s="20">
         <v>4</v>
       </c>
@@ -3093,62 +3430,62 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="57" t="s">
+      <c r="A10" s="74" t="s">
         <v>28</v>
       </c>
-      <c r="B10" s="57"/>
-      <c r="C10" s="57"/>
-      <c r="D10" s="57"/>
-      <c r="E10" s="57"/>
-      <c r="F10" s="57"/>
-      <c r="G10" s="57"/>
-      <c r="H10" s="57"/>
-      <c r="I10" s="57"/>
-      <c r="J10" s="57"/>
-      <c r="K10" s="57"/>
-      <c r="L10" s="57"/>
-      <c r="M10" s="57"/>
-      <c r="N10" s="57"/>
-      <c r="O10" s="57"/>
+      <c r="B10" s="74"/>
+      <c r="C10" s="74"/>
+      <c r="D10" s="74"/>
+      <c r="E10" s="74"/>
+      <c r="F10" s="74"/>
+      <c r="G10" s="74"/>
+      <c r="H10" s="74"/>
+      <c r="I10" s="74"/>
+      <c r="J10" s="74"/>
+      <c r="K10" s="74"/>
+      <c r="L10" s="74"/>
+      <c r="M10" s="74"/>
+      <c r="N10" s="74"/>
+      <c r="O10" s="74"/>
     </row>
     <row r="11" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="54" t="s">
+      <c r="A11" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="55"/>
-      <c r="C11" s="54" t="s">
+      <c r="B11" s="66"/>
+      <c r="C11" s="73" t="s">
         <v>6</v>
       </c>
-      <c r="D11" s="55"/>
-      <c r="E11" s="53" t="s">
+      <c r="D11" s="66"/>
+      <c r="E11" s="65" t="s">
         <v>35</v>
       </c>
-      <c r="F11" s="55"/>
-      <c r="G11" s="53" t="s">
+      <c r="F11" s="66"/>
+      <c r="G11" s="65" t="s">
         <v>31</v>
       </c>
-      <c r="H11" s="55"/>
-      <c r="I11" s="53" t="s">
+      <c r="H11" s="66"/>
+      <c r="I11" s="65" t="s">
         <v>36</v>
       </c>
-      <c r="J11" s="55"/>
-      <c r="K11" s="54" t="s">
+      <c r="J11" s="66"/>
+      <c r="K11" s="73" t="s">
         <v>29</v>
       </c>
-      <c r="L11" s="55"/>
-      <c r="M11" s="53" t="s">
+      <c r="L11" s="66"/>
+      <c r="M11" s="65" t="s">
         <v>37</v>
       </c>
-      <c r="N11" s="55"/>
-      <c r="O11" s="53" t="s">
+      <c r="N11" s="66"/>
+      <c r="O11" s="65" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="57" t="s">
+      <c r="A12" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="58"/>
+      <c r="B12" s="75"/>
       <c r="C12" s="5" t="s">
         <v>2</v>
       </c>
@@ -3185,10 +3522,10 @@
       <c r="N12" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="O12" s="56"/>
+      <c r="O12" s="77"/>
     </row>
     <row r="13" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="50" t="s">
+      <c r="A13" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="18">
@@ -3227,7 +3564,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="67"/>
+      <c r="A14" s="76"/>
       <c r="B14" s="19">
         <v>1</v>
       </c>
@@ -3272,7 +3609,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
+      <c r="A15" s="76"/>
       <c r="B15" s="19">
         <v>2</v>
       </c>
@@ -3317,7 +3654,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="67"/>
+      <c r="A16" s="76"/>
       <c r="B16" s="19">
         <v>3</v>
       </c>
@@ -3362,7 +3699,7 @@
       </c>
     </row>
     <row r="17" spans="1:15" ht="17.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="52"/>
+      <c r="A17" s="72"/>
       <c r="B17" s="20">
         <v>4</v>
       </c>
@@ -3408,6 +3745,12 @@
     </row>
   </sheetData>
   <mergeCells count="22">
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="O2:O3"/>
+    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="M2:N2"/>
+    <mergeCell ref="M11:N11"/>
     <mergeCell ref="A1:O1"/>
     <mergeCell ref="A10:O10"/>
     <mergeCell ref="A13:A17"/>
@@ -3424,15 +3767,9 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="O11:O12"/>
     <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="O2:O3"/>
-    <mergeCell ref="K11:L11"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="M2:N2"/>
-    <mergeCell ref="M11:N11"/>
   </mergeCells>
   <conditionalFormatting sqref="O4:O8">
-    <cfRule type="cellIs" dxfId="56" priority="2" operator="lessThan">
+    <cfRule type="cellIs" dxfId="88" priority="2" operator="lessThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -3455,23 +3792,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A1" s="68" t="s">
+      <c r="A1" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="70" t="s">
+      <c r="C1" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="D1" s="71"/>
-      <c r="E1" s="71"/>
-      <c r="F1" s="71"/>
-      <c r="G1" s="72"/>
+      <c r="D1" s="81"/>
+      <c r="E1" s="81"/>
+      <c r="F1" s="81"/>
+      <c r="G1" s="82"/>
     </row>
     <row r="2" spans="1:21" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="69"/>
-      <c r="B2" s="69"/>
+      <c r="A2" s="79"/>
+      <c r="B2" s="79"/>
       <c r="C2" s="1" t="s">
         <v>18</v>
       </c>
@@ -3534,23 +3871,23 @@
         <v>2.5419999999999998</v>
       </c>
       <c r="J4">
-        <f>C4/C$3</f>
+        <f t="shared" ref="J4:K9" si="0">C4/C$3</f>
         <v>1.114957264957265</v>
       </c>
       <c r="K4">
-        <f>D4/D$3</f>
+        <f t="shared" si="0"/>
         <v>1.0705843729481288</v>
       </c>
       <c r="S4">
-        <f>E4/E$3</f>
+        <f t="shared" ref="S4:U9" si="1">E4/E$3</f>
         <v>1.0693861990087685</v>
       </c>
       <c r="T4">
-        <f>F4/F$3</f>
+        <f t="shared" si="1"/>
         <v>1.9703989703989702</v>
       </c>
       <c r="U4">
-        <f>G4/G$3</f>
+        <f t="shared" si="1"/>
         <v>1.4609195402298849</v>
       </c>
     </row>
@@ -3577,23 +3914,23 @@
         <v>2.488</v>
       </c>
       <c r="J5" t="e">
-        <f>C5/C$3</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="K5">
-        <f>D5/D$3</f>
+        <f t="shared" si="0"/>
         <v>1.0469468154957322</v>
       </c>
       <c r="S5">
-        <f>E5/E$3</f>
+        <f t="shared" si="1"/>
         <v>1.0152497140678611</v>
       </c>
       <c r="T5">
-        <f>F5/F$3</f>
+        <f t="shared" si="1"/>
         <v>1.9221364221364221</v>
       </c>
       <c r="U5">
-        <f>G5/G$3</f>
+        <f t="shared" si="1"/>
         <v>1.4298850574712643</v>
       </c>
     </row>
@@ -3620,23 +3957,23 @@
         <v>1.542</v>
       </c>
       <c r="J6">
-        <f>C6/C$3</f>
+        <f t="shared" si="0"/>
         <v>0.95128205128205134</v>
       </c>
       <c r="K6">
-        <f>D6/D$3</f>
+        <f t="shared" si="0"/>
         <v>0.91891004596191728</v>
       </c>
       <c r="S6">
-        <f>E6/E$3</f>
+        <f t="shared" si="1"/>
         <v>0.94433854365230641</v>
       </c>
       <c r="T6">
-        <f>F6/F$3</f>
+        <f t="shared" si="1"/>
         <v>1.1190476190476191</v>
       </c>
       <c r="U6">
-        <f>G6/G$3</f>
+        <f t="shared" si="1"/>
         <v>0.88620689655172413</v>
       </c>
     </row>
@@ -3663,23 +4000,23 @@
         <v>1.59</v>
       </c>
       <c r="J7" t="e">
-        <f>C7/C$3</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="K7">
-        <f>D7/D$3</f>
+        <f t="shared" si="0"/>
         <v>0.95535128036769545</v>
       </c>
       <c r="S7">
-        <f>E7/E$3</f>
+        <f t="shared" si="1"/>
         <v>0.90964544414792214</v>
       </c>
       <c r="T7">
-        <f>F7/F$3</f>
+        <f t="shared" si="1"/>
         <v>1.1184041184041185</v>
       </c>
       <c r="U7">
-        <f>G7/G$3</f>
+        <f t="shared" si="1"/>
         <v>0.91379310344827591</v>
       </c>
     </row>
@@ -3706,23 +4043,23 @@
         <v>1.8560000000000001</v>
       </c>
       <c r="J8">
-        <f>C8/C$3</f>
+        <f t="shared" si="0"/>
         <v>0.87264957264957266</v>
       </c>
       <c r="K8">
-        <f>D8/D$3</f>
+        <f t="shared" si="0"/>
         <v>0.68089297439264607</v>
       </c>
       <c r="S8">
-        <f>E8/E$3</f>
+        <f t="shared" si="1"/>
         <v>0.85741517346549745</v>
       </c>
       <c r="T8">
-        <f>F8/F$3</f>
+        <f t="shared" si="1"/>
         <v>0.88095238095238093</v>
       </c>
       <c r="U8">
-        <f>G8/G$3</f>
+        <f t="shared" si="1"/>
         <v>1.0666666666666667</v>
       </c>
     </row>
@@ -3749,45 +4086,45 @@
         <v>1.9390000000000001</v>
       </c>
       <c r="J9" t="e">
-        <f>C9/C$3</f>
+        <f t="shared" si="0"/>
         <v>#VALUE!</v>
       </c>
       <c r="K9">
-        <f>D9/D$3</f>
+        <f t="shared" si="0"/>
         <v>0.71634931057124096</v>
       </c>
       <c r="S9">
-        <f>E9/E$3</f>
+        <f t="shared" si="1"/>
         <v>0.86313381624094532</v>
       </c>
       <c r="T9">
-        <f>F9/F$3</f>
+        <f t="shared" si="1"/>
         <v>0.79665379665379665</v>
       </c>
       <c r="U9">
-        <f>G9/G$3</f>
+        <f t="shared" si="1"/>
         <v>1.1143678160919541</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="68" t="s">
+      <c r="A12" s="78" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="78" t="s">
         <v>4</v>
       </c>
-      <c r="C12" s="70" t="s">
+      <c r="C12" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="71"/>
-      <c r="E12" s="71"/>
-      <c r="F12" s="71"/>
-      <c r="G12" s="72"/>
+      <c r="D12" s="81"/>
+      <c r="E12" s="81"/>
+      <c r="F12" s="81"/>
+      <c r="G12" s="82"/>
     </row>
     <row r="13" spans="1:21" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="69"/>
-      <c r="B13" s="69"/>
+      <c r="A13" s="79"/>
+      <c r="B13" s="79"/>
       <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
@@ -3850,23 +4187,23 @@
         <v>3.105</v>
       </c>
       <c r="J15">
-        <f>C15/C$14</f>
+        <f t="shared" ref="J15:K20" si="2">C15/C$14</f>
         <v>0.91148531951640777</v>
       </c>
       <c r="K15">
-        <f>D15/D$14</f>
+        <f t="shared" si="2"/>
         <v>1.0308455565142363</v>
       </c>
       <c r="S15">
-        <f>E15/E$14</f>
+        <f t="shared" ref="S15:U20" si="3">E15/E$14</f>
         <v>1.0166002656042497</v>
       </c>
       <c r="T15">
-        <f>F15/F$14</f>
+        <f t="shared" si="3"/>
         <v>1.2928039702233249</v>
       </c>
       <c r="U15">
-        <f>G15/G$14</f>
+        <f t="shared" si="3"/>
         <v>1.6995073891625616</v>
       </c>
     </row>
@@ -3893,23 +4230,23 @@
         <v>3.3119999999999998</v>
       </c>
       <c r="J16" t="e">
-        <f>C16/C$14</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="K16">
-        <f>D16/D$14</f>
+        <f t="shared" si="2"/>
         <v>1.0036669542709231</v>
       </c>
       <c r="S16">
-        <f>E16/E$14</f>
+        <f t="shared" si="3"/>
         <v>1.0411686586985391</v>
       </c>
       <c r="T16">
-        <f>F16/F$14</f>
+        <f t="shared" si="3"/>
         <v>1.4218362282878412</v>
       </c>
       <c r="U16">
-        <f>G16/G$14</f>
+        <f t="shared" si="3"/>
         <v>1.812807881773399</v>
       </c>
     </row>
@@ -3936,23 +4273,23 @@
         <v>2.0939999999999999</v>
       </c>
       <c r="J17">
-        <f>C17/C$14</f>
+        <f t="shared" si="2"/>
         <v>1.8341968911917101</v>
       </c>
       <c r="K17">
-        <f>D17/D$14</f>
+        <f t="shared" si="2"/>
         <v>1.3125539257981018</v>
       </c>
       <c r="S17">
-        <f>E17/E$14</f>
+        <f t="shared" si="3"/>
         <v>1.2549800796812749</v>
       </c>
       <c r="T17">
-        <f>F17/F$14</f>
+        <f t="shared" si="3"/>
         <v>1.2460711331679073</v>
       </c>
       <c r="U17">
-        <f>G17/G$14</f>
+        <f t="shared" si="3"/>
         <v>1.1461412151067323</v>
       </c>
     </row>
@@ -3979,23 +4316,23 @@
         <v>2.1659999999999999</v>
       </c>
       <c r="J18" t="e">
-        <f>C18/C$14</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="K18">
-        <f>D18/D$14</f>
+        <f t="shared" si="2"/>
         <v>1.234253666954271</v>
       </c>
       <c r="S18">
-        <f>E18/E$14</f>
+        <f t="shared" si="3"/>
         <v>1.2200088534749889</v>
       </c>
       <c r="T18">
-        <f>F18/F$14</f>
+        <f t="shared" si="3"/>
         <v>1.325889164598842</v>
       </c>
       <c r="U18">
-        <f>G18/G$14</f>
+        <f t="shared" si="3"/>
         <v>1.1855500821018061</v>
       </c>
     </row>
@@ -4022,23 +4359,23 @@
         <v>2.302</v>
       </c>
       <c r="J19">
-        <f>C19/C$14</f>
+        <f t="shared" si="2"/>
         <v>2.3907599309153715</v>
       </c>
       <c r="K19">
-        <f>D19/D$14</f>
+        <f t="shared" si="2"/>
         <v>1.3004745470232959</v>
       </c>
       <c r="S19">
-        <f>E19/E$14</f>
+        <f t="shared" si="3"/>
         <v>1.0524568393094289</v>
       </c>
       <c r="T19">
-        <f>F19/F$14</f>
+        <f t="shared" si="3"/>
         <v>0.80066170388751023</v>
       </c>
       <c r="U19">
-        <f>G19/G$14</f>
+        <f t="shared" si="3"/>
         <v>1.2599890530925015</v>
       </c>
     </row>
@@ -4065,23 +4402,23 @@
         <v>2.1030000000000002</v>
       </c>
       <c r="J20" t="e">
-        <f>C20/C$14</f>
+        <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
       <c r="K20">
-        <f>D20/D$14</f>
+        <f t="shared" si="2"/>
         <v>1.3004745470232959</v>
       </c>
       <c r="S20">
-        <f>E20/E$14</f>
+        <f t="shared" si="3"/>
         <v>1.0945108455068615</v>
       </c>
       <c r="T20">
-        <f>F20/F$14</f>
+        <f t="shared" si="3"/>
         <v>0.86145574855252272</v>
       </c>
       <c r="U20">
-        <f>G20/G$14</f>
+        <f t="shared" si="3"/>
         <v>1.1510673234811166</v>
       </c>
     </row>
@@ -4155,9 +4492,645 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="R13" sqref="R13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" customWidth="1"/>
+    <col min="3" max="9" width="12.28515625" style="83" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="58"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="56"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="66"/>
+      <c r="C3" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1.7888601036269431</v>
+      </c>
+      <c r="D5" s="23">
+        <v>2.1036269430051813</v>
+      </c>
+      <c r="E5" s="23">
+        <v>2.37</v>
+      </c>
+      <c r="F5" s="23">
+        <v>2.38</v>
+      </c>
+      <c r="G5" s="23">
+        <v>1.88</v>
+      </c>
+      <c r="H5" s="23">
+        <v>2.5</v>
+      </c>
+      <c r="I5" s="27">
+        <v>1.91</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="71"/>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
+        <v>1.3</v>
+      </c>
+      <c r="D6" s="27">
+        <v>1.3078084555651424</v>
+      </c>
+      <c r="E6" s="27">
+        <v>1.37</v>
+      </c>
+      <c r="F6" s="27">
+        <v>2.5499999999999998</v>
+      </c>
+      <c r="G6" s="27">
+        <v>1.31</v>
+      </c>
+      <c r="H6" s="27">
+        <v>1.45</v>
+      </c>
+      <c r="I6" s="27">
+        <v>1.32</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="71"/>
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="11">
+        <v>1.19</v>
+      </c>
+      <c r="D7" s="27">
+        <v>1.1567065073041169</v>
+      </c>
+      <c r="E7" s="27">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F7" s="27">
+        <v>2.34</v>
+      </c>
+      <c r="G7" s="27">
+        <v>1.06</v>
+      </c>
+      <c r="H7" s="27">
+        <v>1.24</v>
+      </c>
+      <c r="I7" s="27">
+        <v>1.24</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="71"/>
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1.08</v>
+      </c>
+      <c r="D8" s="27">
+        <v>1.1145574855252274</v>
+      </c>
+      <c r="E8" s="27">
+        <v>1.05</v>
+      </c>
+      <c r="F8" s="27">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="G8" s="27">
+        <v>0.73</v>
+      </c>
+      <c r="H8" s="27">
+        <v>0.89</v>
+      </c>
+      <c r="I8" s="27">
+        <v>1.21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="72"/>
+      <c r="B9" s="14">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15">
+        <v>1.3</v>
+      </c>
+      <c r="D9" s="31">
+        <v>0.98303229337712106</v>
+      </c>
+      <c r="E9" s="31">
+        <v>0.89</v>
+      </c>
+      <c r="F9" s="31">
+        <v>0.83</v>
+      </c>
+      <c r="G9" s="31">
+        <v>1.31</v>
+      </c>
+      <c r="H9" s="31">
+        <v>1.02</v>
+      </c>
+      <c r="I9" s="31">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="62"/>
+      <c r="C11" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="22">
+        <v>0</v>
+      </c>
+      <c r="C13" s="23">
+        <v>2.4490500863557858</v>
+      </c>
+      <c r="D13" s="23">
+        <v>2.5660621761658033</v>
+      </c>
+      <c r="E13" s="23">
+        <v>1.55</v>
+      </c>
+      <c r="F13" s="23">
+        <v>2.04</v>
+      </c>
+      <c r="G13" s="23">
+        <v>1.9831606217616582</v>
+      </c>
+      <c r="H13" s="23">
+        <v>1.9831606217616582</v>
+      </c>
+      <c r="I13" s="23">
+        <v>1.49</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="68"/>
+      <c r="B14" s="26">
+        <v>1</v>
+      </c>
+      <c r="C14" s="27">
+        <v>1.4637618636755823</v>
+      </c>
+      <c r="D14" s="27">
+        <v>1.337144089732528</v>
+      </c>
+      <c r="E14" s="27">
+        <v>1.1499999999999999</v>
+      </c>
+      <c r="F14" s="27">
+        <v>1.41</v>
+      </c>
+      <c r="G14" s="27">
+        <v>1.55</v>
+      </c>
+      <c r="H14" s="27">
+        <v>1.49</v>
+      </c>
+      <c r="I14" s="27">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="68"/>
+      <c r="B15" s="26">
+        <v>2</v>
+      </c>
+      <c r="C15" s="27">
+        <v>1.1861443116423196</v>
+      </c>
+      <c r="D15" s="27">
+        <v>1.0624169986719787</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1.05</v>
+      </c>
+      <c r="F15" s="27">
+        <v>1.38</v>
+      </c>
+      <c r="G15" s="27">
+        <v>1.2060646303674192</v>
+      </c>
+      <c r="H15" s="27">
+        <v>1.32</v>
+      </c>
+      <c r="I15" s="27">
+        <v>0.92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="68"/>
+      <c r="B16" s="26">
+        <v>3</v>
+      </c>
+      <c r="C16" s="27">
+        <v>0.92390405293631095</v>
+      </c>
+      <c r="D16" s="27">
+        <v>0.85856079404466501</v>
+      </c>
+      <c r="E16" s="27">
+        <v>1.27</v>
+      </c>
+      <c r="F16" s="27">
+        <v>1.39</v>
+      </c>
+      <c r="G16" s="27">
+        <v>0.87468982630272951</v>
+      </c>
+      <c r="H16" s="27">
+        <v>1.04</v>
+      </c>
+      <c r="I16" s="27">
+        <v>0.94</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="69"/>
+      <c r="B17" s="30">
+        <v>4</v>
+      </c>
+      <c r="C17" s="31">
+        <v>0.87684729064039413</v>
+      </c>
+      <c r="D17" s="31">
+        <v>1.2583470169677067</v>
+      </c>
+      <c r="E17" s="31">
+        <v>1.63</v>
+      </c>
+      <c r="F17" s="31">
+        <v>0.94</v>
+      </c>
+      <c r="G17" s="31">
+        <v>0.8308702791461412</v>
+      </c>
+      <c r="H17" s="31">
+        <v>1.38</v>
+      </c>
+      <c r="I17" s="31">
+        <v>1.1100000000000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="61"/>
+      <c r="C19" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="64"/>
+      <c r="C20" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="36">
+        <v>0</v>
+      </c>
+      <c r="C21" s="23">
+        <v>2.5794473229706392</v>
+      </c>
+      <c r="D21" s="23">
+        <v>2.493091537132988</v>
+      </c>
+      <c r="E21" s="23">
+        <v>2.0332469775474955</v>
+      </c>
+      <c r="F21" s="23">
+        <v>2.3159999999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="68"/>
+      <c r="B22" s="38">
+        <v>1</v>
+      </c>
+      <c r="C22" s="27">
+        <v>1.3779119930974977</v>
+      </c>
+      <c r="D22" s="27">
+        <v>1.4443485763589301</v>
+      </c>
+      <c r="E22" s="27">
+        <v>1.44</v>
+      </c>
+      <c r="F22" s="27">
+        <v>4.6360000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="68"/>
+      <c r="B23" s="38">
+        <v>2</v>
+      </c>
+      <c r="C23" s="27">
+        <v>1.2841965471447543</v>
+      </c>
+      <c r="D23" s="27">
+        <v>1.3906595838866758</v>
+      </c>
+      <c r="E23" s="27">
+        <v>1.39</v>
+      </c>
+      <c r="F23" s="27">
+        <v>4.5179999999999998</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="68"/>
+      <c r="B24" s="38">
+        <v>3</v>
+      </c>
+      <c r="C24" s="27">
+        <v>1.4731182795698923</v>
+      </c>
+      <c r="D24" s="27">
+        <v>1.8308519437551694</v>
+      </c>
+      <c r="E24" s="27">
+        <v>1.7994210090984284</v>
+      </c>
+      <c r="F24" s="27">
+        <v>2.4180000000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="69"/>
+      <c r="B25" s="40">
+        <v>4</v>
+      </c>
+      <c r="C25" s="31">
+        <v>1.2183908045977012</v>
+      </c>
+      <c r="D25" s="31">
+        <v>1.7772304324028463</v>
+      </c>
+      <c r="E25" s="31">
+        <v>1.6726874657909141</v>
+      </c>
+      <c r="F25" s="31">
+        <v>1.827</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D5 C13:H17 C6:I9 C21:E25 I14:I17">
+    <cfRule type="cellIs" dxfId="87" priority="17" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="86" priority="18" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="85" priority="15" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="84" priority="16" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="83" priority="13" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="82" priority="14" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="81" priority="11" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="80" priority="12" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="cellIs" dxfId="79" priority="9" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="78" priority="10" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="77" priority="7" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="76" priority="8" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="75" priority="5" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="74" priority="6" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="73" priority="1" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="72" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
@@ -4169,62 +5142,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="77"/>
+      <c r="A1" s="58"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="53" t="s">
+      <c r="B3" s="66"/>
+      <c r="C3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="59" t="s">
+      <c r="D3" s="66"/>
+      <c r="E3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="59" t="s">
+      <c r="F3" s="61"/>
+      <c r="G3" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="66"/>
-      <c r="I3" s="59" t="s">
+      <c r="H3" s="61"/>
+      <c r="I3" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="59" t="s">
+      <c r="J3" s="61"/>
+      <c r="K3" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="66"/>
-      <c r="M3" s="59" t="s">
+      <c r="L3" s="61"/>
+      <c r="M3" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="66"/>
+      <c r="N3" s="61"/>
       <c r="O3" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="44" t="s">
         <v>42</v>
       </c>
@@ -4264,7 +5237,7 @@
       <c r="O4" s="21"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="7">
@@ -4311,7 +5284,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="4">
         <v>1</v>
       </c>
@@ -4356,7 +5329,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="4">
         <v>2</v>
       </c>
@@ -4401,7 +5374,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="4">
         <v>3</v>
       </c>
@@ -4446,7 +5419,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="14">
         <v>4</v>
       </c>
@@ -4508,40 +5481,40 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="59" t="s">
+      <c r="B11" s="62"/>
+      <c r="C11" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="59" t="s">
+      <c r="D11" s="61"/>
+      <c r="E11" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="66"/>
-      <c r="G11" s="59" t="s">
+      <c r="F11" s="61"/>
+      <c r="G11" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="60"/>
-      <c r="I11" s="59" t="s">
+      <c r="H11" s="62"/>
+      <c r="I11" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="66"/>
-      <c r="K11" s="59" t="s">
+      <c r="J11" s="61"/>
+      <c r="K11" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="66"/>
-      <c r="M11" s="59" t="s">
+      <c r="L11" s="61"/>
+      <c r="M11" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="60"/>
+      <c r="N11" s="62"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="61"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="21" t="s">
         <v>42</v>
       </c>
@@ -4580,7 +5553,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="22">
@@ -4624,7 +5597,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="26">
         <v>1</v>
       </c>
@@ -4666,7 +5639,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="26">
         <v>2</v>
       </c>
@@ -4708,7 +5681,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
+      <c r="A16" s="68"/>
       <c r="B16" s="26">
         <v>3</v>
       </c>
@@ -4750,7 +5723,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="30">
         <v>4</v>
       </c>
@@ -4805,35 +5778,35 @@
       <c r="K18" s="35"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="59" t="s">
+      <c r="B19" s="61"/>
+      <c r="C19" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="59" t="s">
+      <c r="D19" s="61"/>
+      <c r="E19" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="66"/>
-      <c r="G19" s="59" t="s">
+      <c r="F19" s="61"/>
+      <c r="G19" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="66"/>
-      <c r="I19" s="59" t="s">
+      <c r="H19" s="61"/>
+      <c r="I19" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="60"/>
+      <c r="J19" s="62"/>
       <c r="K19" s="45" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="21" t="s">
         <v>42</v>
       </c>
@@ -4863,7 +5836,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="36">
@@ -4898,7 +5871,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
+      <c r="A22" s="68"/>
       <c r="B22" s="38">
         <v>1</v>
       </c>
@@ -4931,7 +5904,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
+      <c r="A23" s="68"/>
       <c r="B23" s="38">
         <v>2</v>
       </c>
@@ -4964,7 +5937,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
+      <c r="A24" s="68"/>
       <c r="B24" s="38">
         <v>3</v>
       </c>
@@ -4997,7 +5970,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="65"/>
+      <c r="A25" s="69"/>
       <c r="B25" s="40">
         <v>4</v>
       </c>
@@ -5031,11 +6004,15 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="C11:D11"/>
-    <mergeCell ref="E11:F11"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="I11:J11"/>
-    <mergeCell ref="K11:L11"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:A25"/>
     <mergeCell ref="M11:N11"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
@@ -5047,85 +6024,81 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
     <mergeCell ref="M3:N3"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="E11:F11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="I11:J11"/>
+    <mergeCell ref="K11:L11"/>
   </mergeCells>
   <conditionalFormatting sqref="E5:F5 C13:N17 C6:O9 C22:J25">
-    <cfRule type="cellIs" dxfId="55" priority="17" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="18" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="71" priority="17" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="70" priority="18" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5:D5">
-    <cfRule type="cellIs" dxfId="53" priority="15" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="52" priority="16" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="69" priority="15" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="68" priority="16" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5:H5">
-    <cfRule type="cellIs" dxfId="51" priority="13" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="50" priority="14" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="67" priority="13" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="66" priority="14" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:J5">
-    <cfRule type="cellIs" dxfId="49" priority="11" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="12" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="65" priority="11" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="64" priority="12" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="M5:N5">
-    <cfRule type="cellIs" dxfId="47" priority="9" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="46" priority="10" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="63" priority="9" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="62" priority="10" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K5:L5">
-    <cfRule type="cellIs" dxfId="45" priority="7" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="44" priority="8" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="61" priority="7" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="60" priority="8" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="C21:D21">
-    <cfRule type="cellIs" dxfId="43" priority="5" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="42" priority="6" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="59" priority="5" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="58" priority="6" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E21:J21">
-    <cfRule type="cellIs" dxfId="41" priority="3" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="40" priority="4" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="57" priority="3" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="56" priority="4" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="O5">
-    <cfRule type="cellIs" dxfId="39" priority="1" operator="lessThan">
-      <formula>1</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="38" priority="2" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="55" priority="1" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="54" priority="2" operator="greaterThan">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -5134,7 +6107,643 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I25"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.85546875" customWidth="1"/>
+    <col min="2" max="2" width="3.28515625" customWidth="1"/>
+    <col min="3" max="9" width="12.42578125" style="83" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="58"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B2" s="56"/>
+      <c r="C2" s="52"/>
+      <c r="D2" s="52"/>
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" s="73" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="66"/>
+      <c r="C3" s="50" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="53" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="53" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="53" t="s">
+        <v>39</v>
+      </c>
+      <c r="G3" s="53" t="s">
+        <v>40</v>
+      </c>
+      <c r="H3" s="53" t="s">
+        <v>29</v>
+      </c>
+      <c r="I3" s="53" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="74" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="75"/>
+      <c r="C4" s="51" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H4" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I4" s="21"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" s="70" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7">
+        <v>0</v>
+      </c>
+      <c r="C5" s="8">
+        <v>0.63504273504273512</v>
+      </c>
+      <c r="D5" s="23">
+        <v>0.72478632478632476</v>
+      </c>
+      <c r="E5" s="23">
+        <v>0.85982905982905988</v>
+      </c>
+      <c r="F5" s="23">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="G5" s="23">
+        <v>0.76</v>
+      </c>
+      <c r="H5" s="23">
+        <v>0.63846153846153852</v>
+      </c>
+      <c r="I5" s="27">
+        <v>1.04</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A6" s="71"/>
+      <c r="B6" s="4">
+        <v>1</v>
+      </c>
+      <c r="C6" s="11">
+        <v>0.68286277084701252</v>
+      </c>
+      <c r="D6" s="27">
+        <v>0.91956664478003947</v>
+      </c>
+      <c r="E6" s="27">
+        <v>0.92744583059750507</v>
+      </c>
+      <c r="F6" s="27">
+        <v>0.63</v>
+      </c>
+      <c r="G6" s="27">
+        <v>0.97</v>
+      </c>
+      <c r="H6" s="27">
+        <v>0.82994090610636906</v>
+      </c>
+      <c r="I6" s="27">
+        <v>0.99</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="71"/>
+      <c r="B7" s="4">
+        <v>2</v>
+      </c>
+      <c r="C7" s="11">
+        <v>0.7941288600838734</v>
+      </c>
+      <c r="D7" s="27">
+        <v>0.96645062905070522</v>
+      </c>
+      <c r="E7" s="27">
+        <v>0.9733130003812428</v>
+      </c>
+      <c r="F7" s="27">
+        <v>0.78</v>
+      </c>
+      <c r="G7" s="27">
+        <v>0.85</v>
+      </c>
+      <c r="H7" s="27">
+        <v>0.97026305756767051</v>
+      </c>
+      <c r="I7" s="27">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="71"/>
+      <c r="B8" s="4">
+        <v>3</v>
+      </c>
+      <c r="C8" s="11">
+        <v>1.4472329472329473</v>
+      </c>
+      <c r="D8" s="27">
+        <v>1.0669240669240669</v>
+      </c>
+      <c r="E8" s="27">
+        <v>1.0360360360360361</v>
+      </c>
+      <c r="F8" s="27">
+        <v>1.41</v>
+      </c>
+      <c r="G8" s="27">
+        <v>1.4</v>
+      </c>
+      <c r="H8" s="27">
+        <v>1.059202059202059</v>
+      </c>
+      <c r="I8" s="27">
+        <v>1.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" s="72"/>
+      <c r="B9" s="14">
+        <v>4</v>
+      </c>
+      <c r="C9" s="15">
+        <v>1.1919540229885057</v>
+      </c>
+      <c r="D9" s="31">
+        <v>0.89942528735632177</v>
+      </c>
+      <c r="E9" s="31">
+        <v>0.89482758620689651</v>
+      </c>
+      <c r="F9" s="31">
+        <v>1.32</v>
+      </c>
+      <c r="G9" s="31">
+        <v>1.7</v>
+      </c>
+      <c r="H9" s="31">
+        <v>0.91264367816091962</v>
+      </c>
+      <c r="I9" s="31">
+        <v>1.1599999999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
+      <c r="G10" s="3"/>
+      <c r="H10" s="3"/>
+      <c r="I10" s="3"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="62"/>
+      <c r="C11" s="53" t="s">
+        <v>12</v>
+      </c>
+      <c r="D11" s="53" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="53" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="53" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" s="53" t="s">
+        <v>11</v>
+      </c>
+      <c r="H11" s="53" t="s">
+        <v>10</v>
+      </c>
+      <c r="I11" s="53" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="63"/>
+      <c r="C12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="G12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="H12" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="I12" s="21" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13" s="22">
+        <v>0</v>
+      </c>
+      <c r="C13" s="23">
+        <v>0.52991452991452992</v>
+      </c>
+      <c r="D13" s="23">
+        <v>0.67222222222222228</v>
+      </c>
+      <c r="E13" s="23">
+        <v>0.71111111111111114</v>
+      </c>
+      <c r="F13" s="23">
+        <v>0.49658119658119659</v>
+      </c>
+      <c r="G13" s="23">
+        <v>0.70940170940170899</v>
+      </c>
+      <c r="H13" s="23">
+        <v>0.70940170940170943</v>
+      </c>
+      <c r="I13" s="23">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="68"/>
+      <c r="B14" s="26">
+        <v>1</v>
+      </c>
+      <c r="C14" s="27">
+        <v>0.75640183847669074</v>
+      </c>
+      <c r="D14" s="27">
+        <v>0.7383453709783323</v>
+      </c>
+      <c r="E14" s="27">
+        <v>0.98522652659225218</v>
+      </c>
+      <c r="F14" s="27">
+        <v>0.8479973736047276</v>
+      </c>
+      <c r="G14" s="27">
+        <v>0.99179251477347341</v>
+      </c>
+      <c r="H14" s="27">
+        <v>1.0022980958634276</v>
+      </c>
+      <c r="I14" s="27">
+        <v>1.29</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A15" s="68"/>
+      <c r="B15" s="26">
+        <v>2</v>
+      </c>
+      <c r="C15" s="27">
+        <v>0.81319100266869992</v>
+      </c>
+      <c r="D15" s="27">
+        <v>0.87914601601219977</v>
+      </c>
+      <c r="E15" s="27">
+        <v>1.0022874571101792</v>
+      </c>
+      <c r="F15" s="27">
+        <v>0.98665650019062134</v>
+      </c>
+      <c r="G15" s="27">
+        <v>0.91002668699961864</v>
+      </c>
+      <c r="H15" s="27">
+        <v>0.88067098741898586</v>
+      </c>
+      <c r="I15" s="27">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A16" s="68"/>
+      <c r="B16" s="26">
+        <v>3</v>
+      </c>
+      <c r="C16" s="27">
+        <v>1.231016731016731</v>
+      </c>
+      <c r="D16" s="27">
+        <v>0.90990990990990983</v>
+      </c>
+      <c r="E16" s="27">
+        <v>1.8088803088803087</v>
+      </c>
+      <c r="F16" s="27">
+        <v>1.5733590733590732</v>
+      </c>
+      <c r="G16" s="27">
+        <v>1.1917631917631917</v>
+      </c>
+      <c r="H16" s="27">
+        <v>1.1184041184041185</v>
+      </c>
+      <c r="I16" s="27">
+        <v>2.76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17" s="69"/>
+      <c r="B17" s="30">
+        <v>4</v>
+      </c>
+      <c r="C17" s="31">
+        <v>1.1724137931034484</v>
+      </c>
+      <c r="D17" s="31">
+        <v>1.0321839080459771</v>
+      </c>
+      <c r="E17" s="31">
+        <v>1.407471264367816</v>
+      </c>
+      <c r="F17" s="31">
+        <v>1.1787356321839082</v>
+      </c>
+      <c r="G17" s="31">
+        <v>1.0695402298850574</v>
+      </c>
+      <c r="H17" s="31">
+        <v>1.407471264367816</v>
+      </c>
+      <c r="I17" s="31">
+        <v>2.4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18" s="34"/>
+      <c r="B18" s="35"/>
+      <c r="C18" s="34"/>
+      <c r="D18" s="34"/>
+      <c r="E18" s="34"/>
+      <c r="F18" s="34"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19" s="62" t="s">
+        <v>7</v>
+      </c>
+      <c r="B19" s="61"/>
+      <c r="C19" s="53" t="s">
+        <v>32</v>
+      </c>
+      <c r="D19" s="53" t="s">
+        <v>33</v>
+      </c>
+      <c r="E19" s="53" t="s">
+        <v>34</v>
+      </c>
+      <c r="F19" s="53" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20" s="63" t="s">
+        <v>4</v>
+      </c>
+      <c r="B20" s="64"/>
+      <c r="C20" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="D20" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="F20" s="21" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21" s="67" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21" s="36">
+        <v>0</v>
+      </c>
+      <c r="C21" s="23">
+        <v>1.43</v>
+      </c>
+      <c r="D21" s="23">
+        <v>1.176923076923077</v>
+      </c>
+      <c r="E21" s="23">
+        <v>0.81410256410256421</v>
+      </c>
+      <c r="F21" s="23">
+        <v>2.34</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22" s="68"/>
+      <c r="B22" s="38">
+        <v>1</v>
+      </c>
+      <c r="C22" s="27">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="D22" s="27">
+        <v>1.1631648063033488</v>
+      </c>
+      <c r="E22" s="27">
+        <v>0.95272488509520692</v>
+      </c>
+      <c r="F22" s="27">
+        <v>3.0459999999999998</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23" s="68"/>
+      <c r="B23" s="38">
+        <v>2</v>
+      </c>
+      <c r="C23" s="27">
+        <v>1.31</v>
+      </c>
+      <c r="D23" s="27">
+        <v>1.361418223408311</v>
+      </c>
+      <c r="E23" s="27">
+        <v>1.1765154403354936</v>
+      </c>
+      <c r="F23" s="27">
+        <v>2.6230000000000002</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24" s="68"/>
+      <c r="B24" s="38">
+        <v>3</v>
+      </c>
+      <c r="C24" s="27">
+        <v>1.3783783783783783</v>
+      </c>
+      <c r="D24" s="27">
+        <v>1.3487773487773489</v>
+      </c>
+      <c r="E24" s="27">
+        <v>1.1930501930501931</v>
+      </c>
+      <c r="F24" s="27">
+        <v>1.554</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A25" s="69"/>
+      <c r="B25" s="40">
+        <v>4</v>
+      </c>
+      <c r="C25" s="31">
+        <v>1.3356321839080458</v>
+      </c>
+      <c r="D25" s="31">
+        <v>1.3137931034482759</v>
+      </c>
+      <c r="E25" s="31">
+        <v>1.0626436781609194</v>
+      </c>
+      <c r="F25" s="31">
+        <v>1.74</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="A5:A9"/>
+    <mergeCell ref="A11:B11"/>
+    <mergeCell ref="A3:B3"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D5 C13:H17 C6:I9 C21:E25 I14:I17">
+    <cfRule type="cellIs" dxfId="53" priority="17" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="52" priority="18" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C5">
+    <cfRule type="cellIs" dxfId="51" priority="15" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="50" priority="16" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" dxfId="49" priority="13" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="48" priority="14" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F5">
+    <cfRule type="cellIs" dxfId="47" priority="11" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="46" priority="12" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="H5">
+    <cfRule type="cellIs" dxfId="45" priority="9" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="44" priority="10" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="G5">
+    <cfRule type="cellIs" dxfId="43" priority="7" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="42" priority="8" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I13">
+    <cfRule type="cellIs" dxfId="41" priority="5" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="40" priority="6" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I5">
+    <cfRule type="cellIs" dxfId="39" priority="1" operator="lessThan">
+      <formula>1</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="38" priority="2" operator="greaterThan">
+      <formula>1</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O25"/>
   <sheetViews>
@@ -5150,62 +6759,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A1" s="77"/>
+      <c r="A1" s="58"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
-      <c r="M2" s="75"/>
-      <c r="N2" s="75"/>
-      <c r="O2" s="75"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="56"/>
+      <c r="N2" s="56"/>
+      <c r="O2" s="56"/>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="53" t="s">
+      <c r="B3" s="66"/>
+      <c r="C3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="59" t="s">
+      <c r="D3" s="66"/>
+      <c r="E3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="59" t="s">
+      <c r="F3" s="61"/>
+      <c r="G3" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="66"/>
-      <c r="I3" s="59" t="s">
+      <c r="H3" s="61"/>
+      <c r="I3" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="59" t="s">
+      <c r="J3" s="61"/>
+      <c r="K3" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="66"/>
-      <c r="M3" s="59" t="s">
+      <c r="L3" s="61"/>
+      <c r="M3" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="N3" s="66"/>
+      <c r="N3" s="61"/>
       <c r="O3" s="45" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="44" t="s">
         <v>42</v>
       </c>
@@ -5245,7 +6854,7 @@
       <c r="O4" s="21"/>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="7">
@@ -5292,7 +6901,7 @@
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="4">
         <v>1</v>
       </c>
@@ -5337,7 +6946,7 @@
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="4">
         <v>2</v>
       </c>
@@ -5382,7 +6991,7 @@
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="4">
         <v>3</v>
       </c>
@@ -5427,7 +7036,7 @@
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="14">
         <v>4</v>
       </c>
@@ -5489,40 +7098,40 @@
       <c r="O10" s="4"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="59" t="s">
+      <c r="B11" s="62"/>
+      <c r="C11" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="D11" s="66"/>
-      <c r="E11" s="59" t="s">
+      <c r="D11" s="61"/>
+      <c r="E11" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="66"/>
-      <c r="G11" s="59" t="s">
+      <c r="F11" s="61"/>
+      <c r="G11" s="60" t="s">
         <v>6</v>
       </c>
-      <c r="H11" s="60"/>
-      <c r="I11" s="59" t="s">
+      <c r="H11" s="62"/>
+      <c r="I11" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="J11" s="66"/>
-      <c r="K11" s="59" t="s">
+      <c r="J11" s="61"/>
+      <c r="K11" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="L11" s="66"/>
-      <c r="M11" s="59" t="s">
+      <c r="L11" s="61"/>
+      <c r="M11" s="60" t="s">
         <v>10</v>
       </c>
-      <c r="N11" s="60"/>
+      <c r="N11" s="62"/>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="61"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="21" t="s">
         <v>42</v>
       </c>
@@ -5561,7 +7170,7 @@
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="22">
@@ -5605,7 +7214,7 @@
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="26">
         <v>1</v>
       </c>
@@ -5647,7 +7256,7 @@
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="26">
         <v>2</v>
       </c>
@@ -5689,7 +7298,7 @@
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
+      <c r="A16" s="68"/>
       <c r="B16" s="26">
         <v>3</v>
       </c>
@@ -5731,7 +7340,7 @@
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="30">
         <v>4</v>
       </c>
@@ -5786,35 +7395,35 @@
       <c r="K18" s="35"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="66"/>
-      <c r="C19" s="59" t="s">
+      <c r="B19" s="61"/>
+      <c r="C19" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="66"/>
-      <c r="E19" s="59" t="s">
+      <c r="D19" s="61"/>
+      <c r="E19" s="60" t="s">
         <v>32</v>
       </c>
-      <c r="F19" s="66"/>
-      <c r="G19" s="59" t="s">
+      <c r="F19" s="61"/>
+      <c r="G19" s="60" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="66"/>
-      <c r="I19" s="59" t="s">
+      <c r="H19" s="61"/>
+      <c r="I19" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="J19" s="60"/>
+      <c r="J19" s="62"/>
       <c r="K19" s="45" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="21" t="s">
         <v>42</v>
       </c>
@@ -5844,7 +7453,7 @@
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="36">
@@ -5879,7 +7488,7 @@
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
+      <c r="A22" s="68"/>
       <c r="B22" s="38">
         <v>1</v>
       </c>
@@ -5912,7 +7521,7 @@
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
+      <c r="A23" s="68"/>
       <c r="B23" s="38">
         <v>2</v>
       </c>
@@ -5945,7 +7554,7 @@
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
+      <c r="A24" s="68"/>
       <c r="B24" s="38">
         <v>3</v>
       </c>
@@ -5978,7 +7587,7 @@
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A25" s="65"/>
+      <c r="A25" s="69"/>
       <c r="B25" s="40">
         <v>4</v>
       </c>
@@ -6012,15 +7621,6 @@
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="I19:J19"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:A25"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="A19:B19"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="E19:F19"/>
-    <mergeCell ref="G19:H19"/>
     <mergeCell ref="M3:N3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:A9"/>
@@ -6037,6 +7637,15 @@
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="K3:L3"/>
+    <mergeCell ref="I19:J19"/>
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:A25"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="A19:B19"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="E19:F19"/>
+    <mergeCell ref="G19:H19"/>
   </mergeCells>
   <conditionalFormatting sqref="E5:F5 C13:N17 C6:O9 C22:J25">
     <cfRule type="cellIs" dxfId="37" priority="17" operator="lessThan">
@@ -6115,64 +7724,64 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="77"/>
+      <c r="A1" s="58"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B2" s="75"/>
-      <c r="C2" s="75"/>
-      <c r="D2" s="75"/>
-      <c r="E2" s="75"/>
-      <c r="F2" s="75"/>
-      <c r="G2" s="75"/>
-      <c r="H2" s="75"/>
-      <c r="I2" s="75"/>
-      <c r="J2" s="75"/>
-      <c r="K2" s="75"/>
-      <c r="L2" s="75"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="54" t="s">
+      <c r="A3" s="73" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="55"/>
-      <c r="C3" s="53" t="s">
+      <c r="B3" s="66"/>
+      <c r="C3" s="65" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="55"/>
-      <c r="E3" s="59" t="s">
+      <c r="D3" s="66"/>
+      <c r="E3" s="60" t="s">
         <v>15</v>
       </c>
-      <c r="F3" s="66"/>
-      <c r="G3" s="59" t="s">
+      <c r="F3" s="61"/>
+      <c r="G3" s="60" t="s">
         <v>14</v>
       </c>
-      <c r="H3" s="66"/>
-      <c r="I3" s="59" t="s">
+      <c r="H3" s="61"/>
+      <c r="I3" s="60" t="s">
         <v>39</v>
       </c>
-      <c r="J3" s="66"/>
-      <c r="K3" s="59" t="s">
+      <c r="J3" s="61"/>
+      <c r="K3" s="60" t="s">
         <v>40</v>
       </c>
-      <c r="L3" s="60"/>
-      <c r="M3" s="78"/>
+      <c r="L3" s="62"/>
+      <c r="M3" s="59"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="57" t="s">
+      <c r="A4" s="74" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="58"/>
+      <c r="B4" s="75"/>
       <c r="C4" s="44" t="s">
         <v>42</v>
       </c>
@@ -6203,10 +7812,10 @@
       <c r="L4" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="M4" s="78"/>
+      <c r="M4" s="59"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="50" t="s">
+      <c r="A5" s="70" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="7">
@@ -6242,10 +7851,10 @@
       <c r="L5" s="24">
         <v>3.8845829960427798</v>
       </c>
-      <c r="M5" s="78"/>
+      <c r="M5" s="59"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="51"/>
+      <c r="A6" s="71"/>
       <c r="B6" s="4">
         <v>1</v>
       </c>
@@ -6279,10 +7888,10 @@
       <c r="L6" s="28">
         <v>2.071405943152814</v>
       </c>
-      <c r="M6" s="78"/>
+      <c r="M6" s="59"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="51"/>
+      <c r="A7" s="71"/>
       <c r="B7" s="4">
         <v>2</v>
       </c>
@@ -6316,10 +7925,10 @@
       <c r="L7" s="28">
         <v>1.659201924928466</v>
       </c>
-      <c r="M7" s="78"/>
+      <c r="M7" s="59"/>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="51"/>
+      <c r="A8" s="71"/>
       <c r="B8" s="4">
         <v>3</v>
       </c>
@@ -6353,10 +7962,10 @@
       <c r="L8" s="28">
         <v>5.7265979128839879</v>
       </c>
-      <c r="M8" s="78"/>
+      <c r="M8" s="59"/>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="52"/>
+      <c r="A9" s="72"/>
       <c r="B9" s="14">
         <v>4</v>
       </c>
@@ -6390,7 +7999,7 @@
       <c r="L9" s="32">
         <v>2.2107446626459542</v>
       </c>
-      <c r="M9" s="78"/>
+      <c r="M9" s="59"/>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="3"/>
@@ -6407,18 +8016,18 @@
       <c r="L10" s="4"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="60" t="s">
+      <c r="A11" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="60"/>
-      <c r="C11" s="59" t="s">
+      <c r="B11" s="62"/>
+      <c r="C11" s="60" t="s">
         <v>29</v>
       </c>
-      <c r="D11" s="60"/>
-      <c r="E11" s="59" t="s">
+      <c r="D11" s="62"/>
+      <c r="E11" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="F11" s="66"/>
+      <c r="F11" s="61"/>
       <c r="G11" s="45" t="s">
         <v>31</v>
       </c>
@@ -6431,13 +8040,13 @@
         <v>9</v>
       </c>
       <c r="L11" s="46"/>
-      <c r="M11" s="78"/>
+      <c r="M11" s="59"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="61" t="s">
+      <c r="A12" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B12" s="61"/>
+      <c r="B12" s="63"/>
       <c r="C12" s="21" t="s">
         <v>42</v>
       </c>
@@ -6468,10 +8077,10 @@
       <c r="L12" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="M12" s="78"/>
+      <c r="M12" s="59"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="63" t="s">
+      <c r="A13" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B13" s="22">
@@ -6507,10 +8116,10 @@
       <c r="L13" s="24">
         <v>4.1628276407067508</v>
       </c>
-      <c r="M13" s="78"/>
+      <c r="M13" s="59"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="64"/>
+      <c r="A14" s="68"/>
       <c r="B14" s="26">
         <v>1</v>
       </c>
@@ -6541,13 +8150,13 @@
       <c r="K14" s="27">
         <v>1.1520286719303969</v>
       </c>
-      <c r="L14" s="74">
+      <c r="L14" s="55">
         <v>1.161882182612745</v>
       </c>
-      <c r="M14" s="78"/>
+      <c r="M14" s="59"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="64"/>
+      <c r="A15" s="68"/>
       <c r="B15" s="26">
         <v>2</v>
       </c>
@@ -6578,13 +8187,13 @@
       <c r="K15" s="27">
         <v>1.033001894804729</v>
       </c>
-      <c r="L15" s="74">
+      <c r="L15" s="55">
         <v>1.0231896685423501</v>
       </c>
-      <c r="M15" s="78"/>
+      <c r="M15" s="59"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="64"/>
+      <c r="A16" s="68"/>
       <c r="B16" s="26">
         <v>3</v>
       </c>
@@ -6615,13 +8224,13 @@
       <c r="K16" s="27">
         <v>1.9546772683171061</v>
       </c>
-      <c r="L16" s="74">
+      <c r="L16" s="55">
         <v>1.9191139957807981</v>
       </c>
-      <c r="M16" s="78"/>
+      <c r="M16" s="59"/>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="65"/>
+      <c r="A17" s="69"/>
       <c r="B17" s="30">
         <v>4</v>
       </c>
@@ -6655,7 +8264,7 @@
       <c r="L17" s="32">
         <v>1.1439427188657061</v>
       </c>
-      <c r="M17" s="78"/>
+      <c r="M17" s="59"/>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
@@ -6669,10 +8278,10 @@
       <c r="I18" s="35"/>
     </row>
     <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="60" t="s">
+      <c r="A19" s="62" t="s">
         <v>7</v>
       </c>
-      <c r="B19" s="66"/>
+      <c r="B19" s="61"/>
       <c r="C19" s="45" t="s">
         <v>11</v>
       </c>
@@ -6681,19 +8290,19 @@
         <v>10</v>
       </c>
       <c r="F19" s="46"/>
-      <c r="G19" s="59" t="s">
+      <c r="G19" s="60" t="s">
         <v>41</v>
       </c>
-      <c r="H19" s="66"/>
+      <c r="H19" s="61"/>
       <c r="I19" s="45" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="61" t="s">
+      <c r="A20" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B20" s="62"/>
+      <c r="B20" s="64"/>
       <c r="C20" s="21" t="s">
         <v>42</v>
       </c>
@@ -6717,7 +8326,7 @@
       </c>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="63" t="s">
+      <c r="A21" s="67" t="s">
         <v>0</v>
       </c>
       <c r="B21" s="36">
@@ -6746,7 +8355,7 @@
       </c>
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="64"/>
+      <c r="A22" s="68"/>
       <c r="B22" s="38">
         <v>1</v>
       </c>
@@ -6773,7 +8382,7 @@
       </c>
     </row>
     <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="64"/>
+      <c r="A23" s="68"/>
       <c r="B23" s="38">
         <v>2</v>
       </c>
@@ -6800,7 +8409,7 @@
       </c>
     </row>
     <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="64"/>
+      <c r="A24" s="68"/>
       <c r="B24" s="38">
         <v>3</v>
       </c>
@@ -6827,7 +8436,7 @@
       </c>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="65"/>
+      <c r="A25" s="69"/>
       <c r="B25" s="40">
         <v>4</v>
       </c>
@@ -6855,6 +8464,8 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="A20:B20"/>
+    <mergeCell ref="A21:A25"/>
     <mergeCell ref="A12:B12"/>
     <mergeCell ref="A13:A17"/>
     <mergeCell ref="A19:B19"/>
@@ -6870,8 +8481,6 @@
     <mergeCell ref="E3:F3"/>
     <mergeCell ref="G3:H3"/>
     <mergeCell ref="I3:J3"/>
-    <mergeCell ref="A20:B20"/>
-    <mergeCell ref="A21:A25"/>
   </mergeCells>
   <conditionalFormatting sqref="C21:F25">
     <cfRule type="cellIs" dxfId="19" priority="1" operator="lessThan">

</xml_diff>